<commit_message>
Ajustes reporte 2 y 3
</commit_message>
<xml_diff>
--- a/templates/plantilla_form2.xlsx
+++ b/templates/plantilla_form2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Marcela\MONITORIA\extension-server\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0235D6-908C-4685-B817-533615ABBEFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3725302-E77E-4FBB-B9F6-5D634B107DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -543,7 +543,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\.m"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -601,6 +601,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1195,7 +1203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1239,49 +1247,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1316,37 +1281,45 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1361,9 +1334,43 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1855,8 +1862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH1002"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K56" sqref="K56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2097,21 +2104,21 @@
       <c r="D7" s="16"/>
       <c r="E7" s="17"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="48" t="s">
+      <c r="G7" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="49"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="48" t="s">
+      <c r="H7" s="60"/>
+      <c r="I7" s="61"/>
+      <c r="J7" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="49"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="48" t="s">
+      <c r="K7" s="60"/>
+      <c r="L7" s="61"/>
+      <c r="M7" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="N7" s="49"/>
-      <c r="O7" s="50"/>
+      <c r="N7" s="60"/>
+      <c r="O7" s="61"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
@@ -2129,21 +2136,21 @@
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="51" t="s">
+      <c r="G8" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="52"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="51" t="s">
+      <c r="H8" s="63"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="52"/>
-      <c r="L8" s="53"/>
-      <c r="M8" s="51" t="s">
+      <c r="K8" s="63"/>
+      <c r="L8" s="64"/>
+      <c r="M8" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="N8" s="52"/>
-      <c r="O8" s="53"/>
+      <c r="N8" s="63"/>
+      <c r="O8" s="64"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
@@ -2191,19 +2198,19 @@
       <c r="AH9" s="1"/>
     </row>
     <row r="10" spans="1:34" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="55" t="s">
+      <c r="B10" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="56" t="s">
+      <c r="C10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="57" t="s">
+      <c r="D10" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="58" t="s">
+      <c r="E10" s="41" t="s">
         <v>12</v>
       </c>
       <c r="I10" s="13"/>
@@ -2215,32 +2222,32 @@
       <c r="O10" s="13"/>
       <c r="P10" s="13"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="37"/>
-      <c r="S10" s="38"/>
-      <c r="T10" s="38"/>
-      <c r="U10" s="38"/>
-      <c r="V10" s="38"/>
-      <c r="W10" s="38"/>
-      <c r="X10" s="38"/>
-      <c r="Y10" s="38"/>
-      <c r="Z10" s="38"/>
-      <c r="AA10" s="38"/>
-      <c r="AB10" s="38"/>
-      <c r="AC10" s="38"/>
-      <c r="AD10" s="38"/>
-      <c r="AE10" s="38"/>
-      <c r="AF10" s="38"/>
-      <c r="AG10" s="38"/>
-      <c r="AH10" s="39"/>
+      <c r="R10" s="56"/>
+      <c r="S10" s="57"/>
+      <c r="T10" s="57"/>
+      <c r="U10" s="57"/>
+      <c r="V10" s="57"/>
+      <c r="W10" s="57"/>
+      <c r="X10" s="57"/>
+      <c r="Y10" s="57"/>
+      <c r="Z10" s="57"/>
+      <c r="AA10" s="57"/>
+      <c r="AB10" s="57"/>
+      <c r="AC10" s="57"/>
+      <c r="AD10" s="57"/>
+      <c r="AE10" s="57"/>
+      <c r="AF10" s="57"/>
+      <c r="AG10" s="57"/>
+      <c r="AH10" s="58"/>
     </row>
     <row r="11" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="59"/>
+      <c r="A11" s="42"/>
       <c r="B11" s="18" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
-      <c r="E11" s="60"/>
+      <c r="E11" s="43"/>
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
@@ -2250,26 +2257,26 @@
       <c r="O11" s="13"/>
       <c r="P11" s="13"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="37"/>
-      <c r="S11" s="38"/>
-      <c r="T11" s="38"/>
-      <c r="U11" s="38"/>
-      <c r="V11" s="38"/>
-      <c r="W11" s="38"/>
-      <c r="X11" s="38"/>
-      <c r="Y11" s="38"/>
-      <c r="Z11" s="38"/>
-      <c r="AA11" s="38"/>
-      <c r="AB11" s="38"/>
-      <c r="AC11" s="38"/>
-      <c r="AD11" s="38"/>
-      <c r="AE11" s="38"/>
-      <c r="AF11" s="38"/>
-      <c r="AG11" s="38"/>
-      <c r="AH11" s="39"/>
+      <c r="R11" s="56"/>
+      <c r="S11" s="57"/>
+      <c r="T11" s="57"/>
+      <c r="U11" s="57"/>
+      <c r="V11" s="57"/>
+      <c r="W11" s="57"/>
+      <c r="X11" s="57"/>
+      <c r="Y11" s="57"/>
+      <c r="Z11" s="57"/>
+      <c r="AA11" s="57"/>
+      <c r="AB11" s="57"/>
+      <c r="AC11" s="57"/>
+      <c r="AD11" s="57"/>
+      <c r="AE11" s="57"/>
+      <c r="AF11" s="57"/>
+      <c r="AG11" s="57"/>
+      <c r="AH11" s="58"/>
     </row>
     <row r="12" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="59"/>
+      <c r="A12" s="42"/>
       <c r="B12" s="22" t="s">
         <v>14</v>
       </c>
@@ -2279,7 +2286,7 @@
       <c r="D12" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="61" t="s">
+      <c r="E12" s="44" t="s">
         <v>17</v>
       </c>
       <c r="I12" s="13"/>
@@ -2291,32 +2298,32 @@
       <c r="O12" s="13"/>
       <c r="P12" s="13"/>
       <c r="Q12" s="1"/>
-      <c r="R12" s="37"/>
-      <c r="S12" s="38"/>
-      <c r="T12" s="38"/>
-      <c r="U12" s="38"/>
-      <c r="V12" s="38"/>
-      <c r="W12" s="38"/>
-      <c r="X12" s="38"/>
-      <c r="Y12" s="38"/>
-      <c r="Z12" s="38"/>
-      <c r="AA12" s="38"/>
-      <c r="AB12" s="38"/>
-      <c r="AC12" s="38"/>
-      <c r="AD12" s="38"/>
-      <c r="AE12" s="38"/>
-      <c r="AF12" s="38"/>
-      <c r="AG12" s="38"/>
-      <c r="AH12" s="39"/>
+      <c r="R12" s="56"/>
+      <c r="S12" s="57"/>
+      <c r="T12" s="57"/>
+      <c r="U12" s="57"/>
+      <c r="V12" s="57"/>
+      <c r="W12" s="57"/>
+      <c r="X12" s="57"/>
+      <c r="Y12" s="57"/>
+      <c r="Z12" s="57"/>
+      <c r="AA12" s="57"/>
+      <c r="AB12" s="57"/>
+      <c r="AC12" s="57"/>
+      <c r="AD12" s="57"/>
+      <c r="AE12" s="57"/>
+      <c r="AF12" s="57"/>
+      <c r="AG12" s="57"/>
+      <c r="AH12" s="58"/>
     </row>
     <row r="13" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="59"/>
+      <c r="A13" s="42"/>
       <c r="B13" s="20" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
-      <c r="E13" s="62"/>
+      <c r="E13" s="45"/>
       <c r="I13" s="13"/>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
@@ -2326,32 +2333,32 @@
       <c r="O13" s="13"/>
       <c r="P13" s="13"/>
       <c r="Q13" s="1"/>
-      <c r="R13" s="37"/>
-      <c r="S13" s="38"/>
-      <c r="T13" s="38"/>
-      <c r="U13" s="38"/>
-      <c r="V13" s="38"/>
-      <c r="W13" s="38"/>
-      <c r="X13" s="38"/>
-      <c r="Y13" s="38"/>
-      <c r="Z13" s="38"/>
-      <c r="AA13" s="38"/>
-      <c r="AB13" s="38"/>
-      <c r="AC13" s="38"/>
-      <c r="AD13" s="38"/>
-      <c r="AE13" s="38"/>
-      <c r="AF13" s="38"/>
-      <c r="AG13" s="38"/>
-      <c r="AH13" s="39"/>
+      <c r="R13" s="56"/>
+      <c r="S13" s="57"/>
+      <c r="T13" s="57"/>
+      <c r="U13" s="57"/>
+      <c r="V13" s="57"/>
+      <c r="W13" s="57"/>
+      <c r="X13" s="57"/>
+      <c r="Y13" s="57"/>
+      <c r="Z13" s="57"/>
+      <c r="AA13" s="57"/>
+      <c r="AB13" s="57"/>
+      <c r="AC13" s="57"/>
+      <c r="AD13" s="57"/>
+      <c r="AE13" s="57"/>
+      <c r="AF13" s="57"/>
+      <c r="AG13" s="57"/>
+      <c r="AH13" s="58"/>
     </row>
     <row r="14" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="59"/>
+      <c r="A14" s="42"/>
       <c r="B14" s="18" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
-      <c r="E14" s="60"/>
+      <c r="E14" s="43"/>
       <c r="I14" s="13"/>
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
@@ -2361,26 +2368,26 @@
       <c r="O14" s="13"/>
       <c r="P14" s="13"/>
       <c r="Q14" s="1"/>
-      <c r="R14" s="37"/>
-      <c r="S14" s="38"/>
-      <c r="T14" s="38"/>
-      <c r="U14" s="38"/>
-      <c r="V14" s="38"/>
-      <c r="W14" s="38"/>
-      <c r="X14" s="38"/>
-      <c r="Y14" s="38"/>
-      <c r="Z14" s="38"/>
-      <c r="AA14" s="38"/>
-      <c r="AB14" s="38"/>
-      <c r="AC14" s="38"/>
-      <c r="AD14" s="38"/>
-      <c r="AE14" s="38"/>
-      <c r="AF14" s="38"/>
-      <c r="AG14" s="38"/>
-      <c r="AH14" s="39"/>
+      <c r="R14" s="56"/>
+      <c r="S14" s="57"/>
+      <c r="T14" s="57"/>
+      <c r="U14" s="57"/>
+      <c r="V14" s="57"/>
+      <c r="W14" s="57"/>
+      <c r="X14" s="57"/>
+      <c r="Y14" s="57"/>
+      <c r="Z14" s="57"/>
+      <c r="AA14" s="57"/>
+      <c r="AB14" s="57"/>
+      <c r="AC14" s="57"/>
+      <c r="AD14" s="57"/>
+      <c r="AE14" s="57"/>
+      <c r="AF14" s="57"/>
+      <c r="AG14" s="57"/>
+      <c r="AH14" s="58"/>
     </row>
     <row r="15" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="63">
+      <c r="A15" s="46">
         <v>1</v>
       </c>
       <c r="B15" s="9" t="s">
@@ -2392,7 +2399,7 @@
       <c r="D15" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="64" t="s">
+      <c r="E15" s="47" t="s">
         <v>23</v>
       </c>
       <c r="I15" s="13"/>
@@ -2404,26 +2411,26 @@
       <c r="O15" s="13"/>
       <c r="P15" s="13"/>
       <c r="Q15" s="1"/>
-      <c r="R15" s="37"/>
-      <c r="S15" s="38"/>
-      <c r="T15" s="38"/>
-      <c r="U15" s="38"/>
-      <c r="V15" s="38"/>
-      <c r="W15" s="38"/>
-      <c r="X15" s="38"/>
-      <c r="Y15" s="38"/>
-      <c r="Z15" s="38"/>
-      <c r="AA15" s="38"/>
-      <c r="AB15" s="38"/>
-      <c r="AC15" s="38"/>
-      <c r="AD15" s="38"/>
-      <c r="AE15" s="38"/>
-      <c r="AF15" s="38"/>
-      <c r="AG15" s="38"/>
-      <c r="AH15" s="39"/>
+      <c r="R15" s="56"/>
+      <c r="S15" s="57"/>
+      <c r="T15" s="57"/>
+      <c r="U15" s="57"/>
+      <c r="V15" s="57"/>
+      <c r="W15" s="57"/>
+      <c r="X15" s="57"/>
+      <c r="Y15" s="57"/>
+      <c r="Z15" s="57"/>
+      <c r="AA15" s="57"/>
+      <c r="AB15" s="57"/>
+      <c r="AC15" s="57"/>
+      <c r="AD15" s="57"/>
+      <c r="AE15" s="57"/>
+      <c r="AF15" s="57"/>
+      <c r="AG15" s="57"/>
+      <c r="AH15" s="58"/>
     </row>
     <row r="16" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="63" t="s">
+      <c r="A16" s="46" t="s">
         <v>24</v>
       </c>
       <c r="B16" s="7" t="s">
@@ -2435,7 +2442,7 @@
       <c r="D16" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="64" t="s">
+      <c r="E16" s="47" t="s">
         <v>28</v>
       </c>
       <c r="I16" s="13"/>
@@ -2447,26 +2454,26 @@
       <c r="O16" s="13"/>
       <c r="P16" s="13"/>
       <c r="Q16" s="2"/>
-      <c r="R16" s="37"/>
-      <c r="S16" s="38"/>
-      <c r="T16" s="38"/>
-      <c r="U16" s="38"/>
-      <c r="V16" s="38"/>
-      <c r="W16" s="38"/>
-      <c r="X16" s="38"/>
-      <c r="Y16" s="38"/>
-      <c r="Z16" s="38"/>
-      <c r="AA16" s="38"/>
-      <c r="AB16" s="38"/>
-      <c r="AC16" s="38"/>
-      <c r="AD16" s="38"/>
-      <c r="AE16" s="38"/>
-      <c r="AF16" s="38"/>
-      <c r="AG16" s="38"/>
-      <c r="AH16" s="39"/>
+      <c r="R16" s="56"/>
+      <c r="S16" s="57"/>
+      <c r="T16" s="57"/>
+      <c r="U16" s="57"/>
+      <c r="V16" s="57"/>
+      <c r="W16" s="57"/>
+      <c r="X16" s="57"/>
+      <c r="Y16" s="57"/>
+      <c r="Z16" s="57"/>
+      <c r="AA16" s="57"/>
+      <c r="AB16" s="57"/>
+      <c r="AC16" s="57"/>
+      <c r="AD16" s="57"/>
+      <c r="AE16" s="57"/>
+      <c r="AF16" s="57"/>
+      <c r="AG16" s="57"/>
+      <c r="AH16" s="58"/>
     </row>
     <row r="17" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="63" t="s">
+      <c r="A17" s="46" t="s">
         <v>29</v>
       </c>
       <c r="B17" s="7" t="s">
@@ -2478,7 +2485,7 @@
       <c r="D17" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="64" t="s">
+      <c r="E17" s="47" t="s">
         <v>33</v>
       </c>
       <c r="I17" s="13"/>
@@ -2490,26 +2497,26 @@
       <c r="O17" s="13"/>
       <c r="P17" s="13"/>
       <c r="Q17" s="2"/>
-      <c r="R17" s="37"/>
-      <c r="S17" s="38"/>
-      <c r="T17" s="38"/>
-      <c r="U17" s="38"/>
-      <c r="V17" s="38"/>
-      <c r="W17" s="38"/>
-      <c r="X17" s="38"/>
-      <c r="Y17" s="38"/>
-      <c r="Z17" s="38"/>
-      <c r="AA17" s="38"/>
-      <c r="AB17" s="38"/>
-      <c r="AC17" s="38"/>
-      <c r="AD17" s="38"/>
-      <c r="AE17" s="38"/>
-      <c r="AF17" s="38"/>
-      <c r="AG17" s="38"/>
-      <c r="AH17" s="39"/>
+      <c r="R17" s="56"/>
+      <c r="S17" s="57"/>
+      <c r="T17" s="57"/>
+      <c r="U17" s="57"/>
+      <c r="V17" s="57"/>
+      <c r="W17" s="57"/>
+      <c r="X17" s="57"/>
+      <c r="Y17" s="57"/>
+      <c r="Z17" s="57"/>
+      <c r="AA17" s="57"/>
+      <c r="AB17" s="57"/>
+      <c r="AC17" s="57"/>
+      <c r="AD17" s="57"/>
+      <c r="AE17" s="57"/>
+      <c r="AF17" s="57"/>
+      <c r="AG17" s="57"/>
+      <c r="AH17" s="58"/>
     </row>
     <row r="18" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="63" t="s">
+      <c r="A18" s="46" t="s">
         <v>34</v>
       </c>
       <c r="B18" s="7" t="s">
@@ -2521,7 +2528,7 @@
       <c r="D18" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="64" t="s">
+      <c r="E18" s="47" t="s">
         <v>38</v>
       </c>
       <c r="I18" s="13"/>
@@ -2533,26 +2540,26 @@
       <c r="O18" s="13"/>
       <c r="P18" s="13"/>
       <c r="Q18" s="2"/>
-      <c r="R18" s="37"/>
-      <c r="S18" s="38"/>
-      <c r="T18" s="38"/>
-      <c r="U18" s="38"/>
-      <c r="V18" s="38"/>
-      <c r="W18" s="38"/>
-      <c r="X18" s="38"/>
-      <c r="Y18" s="38"/>
-      <c r="Z18" s="38"/>
-      <c r="AA18" s="38"/>
-      <c r="AB18" s="38"/>
-      <c r="AC18" s="38"/>
-      <c r="AD18" s="38"/>
-      <c r="AE18" s="38"/>
-      <c r="AF18" s="38"/>
-      <c r="AG18" s="38"/>
-      <c r="AH18" s="39"/>
+      <c r="R18" s="56"/>
+      <c r="S18" s="57"/>
+      <c r="T18" s="57"/>
+      <c r="U18" s="57"/>
+      <c r="V18" s="57"/>
+      <c r="W18" s="57"/>
+      <c r="X18" s="57"/>
+      <c r="Y18" s="57"/>
+      <c r="Z18" s="57"/>
+      <c r="AA18" s="57"/>
+      <c r="AB18" s="57"/>
+      <c r="AC18" s="57"/>
+      <c r="AD18" s="57"/>
+      <c r="AE18" s="57"/>
+      <c r="AF18" s="57"/>
+      <c r="AG18" s="57"/>
+      <c r="AH18" s="58"/>
     </row>
     <row r="19" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="63">
+      <c r="A19" s="46">
         <v>2</v>
       </c>
       <c r="B19" s="7" t="s">
@@ -2564,7 +2571,7 @@
       <c r="D19" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="64" t="s">
+      <c r="E19" s="47" t="s">
         <v>42</v>
       </c>
       <c r="I19" s="13"/>
@@ -2576,26 +2583,26 @@
       <c r="O19" s="13"/>
       <c r="P19" s="13"/>
       <c r="Q19" s="2"/>
-      <c r="R19" s="37"/>
-      <c r="S19" s="38"/>
-      <c r="T19" s="38"/>
-      <c r="U19" s="38"/>
-      <c r="V19" s="38"/>
-      <c r="W19" s="38"/>
-      <c r="X19" s="38"/>
-      <c r="Y19" s="38"/>
-      <c r="Z19" s="38"/>
-      <c r="AA19" s="38"/>
-      <c r="AB19" s="38"/>
-      <c r="AC19" s="38"/>
-      <c r="AD19" s="38"/>
-      <c r="AE19" s="38"/>
-      <c r="AF19" s="38"/>
-      <c r="AG19" s="38"/>
-      <c r="AH19" s="39"/>
+      <c r="R19" s="56"/>
+      <c r="S19" s="57"/>
+      <c r="T19" s="57"/>
+      <c r="U19" s="57"/>
+      <c r="V19" s="57"/>
+      <c r="W19" s="57"/>
+      <c r="X19" s="57"/>
+      <c r="Y19" s="57"/>
+      <c r="Z19" s="57"/>
+      <c r="AA19" s="57"/>
+      <c r="AB19" s="57"/>
+      <c r="AC19" s="57"/>
+      <c r="AD19" s="57"/>
+      <c r="AE19" s="57"/>
+      <c r="AF19" s="57"/>
+      <c r="AG19" s="57"/>
+      <c r="AH19" s="58"/>
     </row>
     <row r="20" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="65" t="s">
+      <c r="A20" s="48" t="s">
         <v>43</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -2607,7 +2614,7 @@
       <c r="D20" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="64" t="s">
+      <c r="E20" s="47" t="s">
         <v>47</v>
       </c>
       <c r="I20" s="13"/>
@@ -2638,7 +2645,7 @@
       <c r="AH20" s="1"/>
     </row>
     <row r="21" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="65" t="s">
+      <c r="A21" s="48" t="s">
         <v>48</v>
       </c>
       <c r="B21" s="7" t="s">
@@ -2650,7 +2657,7 @@
       <c r="D21" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="64" t="s">
+      <c r="E21" s="47" t="s">
         <v>52</v>
       </c>
       <c r="I21" s="13"/>
@@ -2681,7 +2688,7 @@
       <c r="AH21" s="1"/>
     </row>
     <row r="22" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="65" t="s">
+      <c r="A22" s="48" t="s">
         <v>53</v>
       </c>
       <c r="B22" s="7" t="s">
@@ -2693,7 +2700,7 @@
       <c r="D22" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E22" s="64" t="s">
+      <c r="E22" s="47" t="s">
         <v>57</v>
       </c>
       <c r="I22" s="13"/>
@@ -2724,7 +2731,7 @@
       <c r="AH22" s="1"/>
     </row>
     <row r="23" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="63">
+      <c r="A23" s="46">
         <v>3</v>
       </c>
       <c r="B23" s="7" t="s">
@@ -2736,7 +2743,7 @@
       <c r="D23" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E23" s="64" t="s">
+      <c r="E23" s="47" t="s">
         <v>61</v>
       </c>
       <c r="I23" s="13"/>
@@ -2748,26 +2755,26 @@
       <c r="O23" s="13"/>
       <c r="P23" s="13"/>
       <c r="Q23" s="2"/>
-      <c r="R23" s="37"/>
-      <c r="S23" s="38"/>
-      <c r="T23" s="38"/>
-      <c r="U23" s="38"/>
-      <c r="V23" s="38"/>
-      <c r="W23" s="38"/>
-      <c r="X23" s="38"/>
-      <c r="Y23" s="38"/>
-      <c r="Z23" s="38"/>
-      <c r="AA23" s="38"/>
-      <c r="AB23" s="38"/>
-      <c r="AC23" s="38"/>
-      <c r="AD23" s="38"/>
-      <c r="AE23" s="38"/>
-      <c r="AF23" s="38"/>
-      <c r="AG23" s="38"/>
-      <c r="AH23" s="39"/>
+      <c r="R23" s="56"/>
+      <c r="S23" s="57"/>
+      <c r="T23" s="57"/>
+      <c r="U23" s="57"/>
+      <c r="V23" s="57"/>
+      <c r="W23" s="57"/>
+      <c r="X23" s="57"/>
+      <c r="Y23" s="57"/>
+      <c r="Z23" s="57"/>
+      <c r="AA23" s="57"/>
+      <c r="AB23" s="57"/>
+      <c r="AC23" s="57"/>
+      <c r="AD23" s="57"/>
+      <c r="AE23" s="57"/>
+      <c r="AF23" s="57"/>
+      <c r="AG23" s="57"/>
+      <c r="AH23" s="58"/>
     </row>
     <row r="24" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="66">
+      <c r="A24" s="49">
         <v>45660</v>
       </c>
       <c r="B24" s="7" t="s">
@@ -2779,7 +2786,7 @@
       <c r="D24" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E24" s="64" t="s">
+      <c r="E24" s="47" t="s">
         <v>65</v>
       </c>
       <c r="I24" s="13"/>
@@ -2791,26 +2798,26 @@
       <c r="O24" s="13"/>
       <c r="P24" s="13"/>
       <c r="Q24" s="2"/>
-      <c r="R24" s="37"/>
-      <c r="S24" s="38"/>
-      <c r="T24" s="38"/>
-      <c r="U24" s="38"/>
-      <c r="V24" s="38"/>
-      <c r="W24" s="38"/>
-      <c r="X24" s="38"/>
-      <c r="Y24" s="38"/>
-      <c r="Z24" s="38"/>
-      <c r="AA24" s="38"/>
-      <c r="AB24" s="38"/>
-      <c r="AC24" s="38"/>
-      <c r="AD24" s="38"/>
-      <c r="AE24" s="38"/>
-      <c r="AF24" s="38"/>
-      <c r="AG24" s="38"/>
-      <c r="AH24" s="39"/>
+      <c r="R24" s="56"/>
+      <c r="S24" s="57"/>
+      <c r="T24" s="57"/>
+      <c r="U24" s="57"/>
+      <c r="V24" s="57"/>
+      <c r="W24" s="57"/>
+      <c r="X24" s="57"/>
+      <c r="Y24" s="57"/>
+      <c r="Z24" s="57"/>
+      <c r="AA24" s="57"/>
+      <c r="AB24" s="57"/>
+      <c r="AC24" s="57"/>
+      <c r="AD24" s="57"/>
+      <c r="AE24" s="57"/>
+      <c r="AF24" s="57"/>
+      <c r="AG24" s="57"/>
+      <c r="AH24" s="58"/>
     </row>
     <row r="25" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="66">
+      <c r="A25" s="49">
         <v>45691</v>
       </c>
       <c r="B25" s="7" t="s">
@@ -2822,7 +2829,7 @@
       <c r="D25" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E25" s="64" t="s">
+      <c r="E25" s="47" t="s">
         <v>69</v>
       </c>
       <c r="I25" s="13"/>
@@ -2834,26 +2841,26 @@
       <c r="O25" s="13"/>
       <c r="P25" s="13"/>
       <c r="Q25" s="2"/>
-      <c r="R25" s="37"/>
-      <c r="S25" s="38"/>
-      <c r="T25" s="38"/>
-      <c r="U25" s="38"/>
-      <c r="V25" s="38"/>
-      <c r="W25" s="38"/>
-      <c r="X25" s="38"/>
-      <c r="Y25" s="38"/>
-      <c r="Z25" s="38"/>
-      <c r="AA25" s="38"/>
-      <c r="AB25" s="38"/>
-      <c r="AC25" s="38"/>
-      <c r="AD25" s="38"/>
-      <c r="AE25" s="38"/>
-      <c r="AF25" s="38"/>
-      <c r="AG25" s="38"/>
-      <c r="AH25" s="39"/>
+      <c r="R25" s="56"/>
+      <c r="S25" s="57"/>
+      <c r="T25" s="57"/>
+      <c r="U25" s="57"/>
+      <c r="V25" s="57"/>
+      <c r="W25" s="57"/>
+      <c r="X25" s="57"/>
+      <c r="Y25" s="57"/>
+      <c r="Z25" s="57"/>
+      <c r="AA25" s="57"/>
+      <c r="AB25" s="57"/>
+      <c r="AC25" s="57"/>
+      <c r="AD25" s="57"/>
+      <c r="AE25" s="57"/>
+      <c r="AF25" s="57"/>
+      <c r="AG25" s="57"/>
+      <c r="AH25" s="58"/>
     </row>
     <row r="26" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="63">
+      <c r="A26" s="46">
         <v>4</v>
       </c>
       <c r="B26" s="7" t="s">
@@ -2865,7 +2872,7 @@
       <c r="D26" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E26" s="64" t="s">
+      <c r="E26" s="47" t="s">
         <v>73</v>
       </c>
       <c r="I26" s="13"/>
@@ -2877,26 +2884,26 @@
       <c r="O26" s="13"/>
       <c r="P26" s="13"/>
       <c r="Q26" s="2"/>
-      <c r="R26" s="37"/>
-      <c r="S26" s="38"/>
-      <c r="T26" s="38"/>
-      <c r="U26" s="38"/>
-      <c r="V26" s="38"/>
-      <c r="W26" s="38"/>
-      <c r="X26" s="38"/>
-      <c r="Y26" s="38"/>
-      <c r="Z26" s="38"/>
-      <c r="AA26" s="38"/>
-      <c r="AB26" s="38"/>
-      <c r="AC26" s="38"/>
-      <c r="AD26" s="38"/>
-      <c r="AE26" s="38"/>
-      <c r="AF26" s="38"/>
-      <c r="AG26" s="38"/>
-      <c r="AH26" s="39"/>
+      <c r="R26" s="56"/>
+      <c r="S26" s="57"/>
+      <c r="T26" s="57"/>
+      <c r="U26" s="57"/>
+      <c r="V26" s="57"/>
+      <c r="W26" s="57"/>
+      <c r="X26" s="57"/>
+      <c r="Y26" s="57"/>
+      <c r="Z26" s="57"/>
+      <c r="AA26" s="57"/>
+      <c r="AB26" s="57"/>
+      <c r="AC26" s="57"/>
+      <c r="AD26" s="57"/>
+      <c r="AE26" s="57"/>
+      <c r="AF26" s="57"/>
+      <c r="AG26" s="57"/>
+      <c r="AH26" s="58"/>
     </row>
     <row r="27" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="66">
+      <c r="A27" s="49">
         <v>45661</v>
       </c>
       <c r="B27" s="7" t="s">
@@ -2908,7 +2915,7 @@
       <c r="D27" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E27" s="64" t="s">
+      <c r="E27" s="47" t="s">
         <v>77</v>
       </c>
       <c r="I27" s="13"/>
@@ -2939,7 +2946,7 @@
       <c r="AH27" s="1"/>
     </row>
     <row r="28" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="66">
+      <c r="A28" s="49">
         <v>45692</v>
       </c>
       <c r="B28" s="7" t="s">
@@ -2951,7 +2958,7 @@
       <c r="D28" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="E28" s="64" t="s">
+      <c r="E28" s="47" t="s">
         <v>81</v>
       </c>
       <c r="I28" s="13"/>
@@ -2982,7 +2989,7 @@
       <c r="AH28" s="1"/>
     </row>
     <row r="29" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="66">
+      <c r="A29" s="49">
         <v>45720</v>
       </c>
       <c r="B29" s="7" t="s">
@@ -2994,7 +3001,7 @@
       <c r="D29" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="E29" s="64" t="s">
+      <c r="E29" s="47" t="s">
         <v>85</v>
       </c>
       <c r="I29" s="13"/>
@@ -3025,7 +3032,7 @@
       <c r="AH29" s="1"/>
     </row>
     <row r="30" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="66">
+      <c r="A30" s="49">
         <v>45751</v>
       </c>
       <c r="B30" s="7" t="s">
@@ -3037,7 +3044,7 @@
       <c r="D30" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="E30" s="64" t="s">
+      <c r="E30" s="47" t="s">
         <v>89</v>
       </c>
       <c r="I30" s="13"/>
@@ -3068,7 +3075,7 @@
       <c r="AH30" s="1"/>
     </row>
     <row r="31" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="63">
+      <c r="A31" s="46">
         <v>5</v>
       </c>
       <c r="B31" s="7" t="s">
@@ -3080,7 +3087,7 @@
       <c r="D31" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="E31" s="64" t="s">
+      <c r="E31" s="47" t="s">
         <v>93</v>
       </c>
       <c r="I31" s="13"/>
@@ -3111,7 +3118,7 @@
       <c r="AH31" s="1"/>
     </row>
     <row r="32" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="66">
+      <c r="A32" s="49">
         <v>45662</v>
       </c>
       <c r="B32" s="7" t="s">
@@ -3123,7 +3130,7 @@
       <c r="D32" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="E32" s="64" t="s">
+      <c r="E32" s="47" t="s">
         <v>97</v>
       </c>
       <c r="I32" s="13"/>
@@ -3154,7 +3161,7 @@
       <c r="AH32" s="1"/>
     </row>
     <row r="33" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="66">
+      <c r="A33" s="49">
         <v>45693</v>
       </c>
       <c r="B33" s="7" t="s">
@@ -3166,7 +3173,7 @@
       <c r="D33" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="E33" s="64" t="s">
+      <c r="E33" s="47" t="s">
         <v>101</v>
       </c>
       <c r="I33" s="13"/>
@@ -3197,7 +3204,7 @@
       <c r="AH33" s="1"/>
     </row>
     <row r="34" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="66">
+      <c r="A34" s="49">
         <v>45721</v>
       </c>
       <c r="B34" s="7" t="s">
@@ -3209,7 +3216,7 @@
       <c r="D34" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="E34" s="64" t="s">
+      <c r="E34" s="47" t="s">
         <v>105</v>
       </c>
       <c r="I34" s="13"/>
@@ -3240,7 +3247,7 @@
       <c r="AH34" s="1"/>
     </row>
     <row r="35" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="63">
+      <c r="A35" s="46">
         <v>6</v>
       </c>
       <c r="B35" s="7" t="s">
@@ -3252,7 +3259,7 @@
       <c r="D35" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="E35" s="64" t="s">
+      <c r="E35" s="47" t="s">
         <v>109</v>
       </c>
       <c r="I35" s="13"/>
@@ -3283,7 +3290,7 @@
       <c r="AH35" s="1"/>
     </row>
     <row r="36" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="66">
+      <c r="A36" s="49">
         <v>45663</v>
       </c>
       <c r="B36" s="7" t="s">
@@ -3295,7 +3302,7 @@
       <c r="D36" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="E36" s="64" t="s">
+      <c r="E36" s="47" t="s">
         <v>113</v>
       </c>
       <c r="I36" s="13"/>
@@ -3326,7 +3333,7 @@
       <c r="AH36" s="1"/>
     </row>
     <row r="37" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="66">
+      <c r="A37" s="49">
         <v>45694</v>
       </c>
       <c r="B37" s="7" t="s">
@@ -3338,7 +3345,7 @@
       <c r="D37" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="E37" s="64" t="s">
+      <c r="E37" s="47" t="s">
         <v>117</v>
       </c>
       <c r="I37" s="13"/>
@@ -3369,7 +3376,7 @@
       <c r="AH37" s="1"/>
     </row>
     <row r="38" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="63">
+      <c r="A38" s="46">
         <v>7</v>
       </c>
       <c r="B38" s="7" t="s">
@@ -3381,7 +3388,7 @@
       <c r="D38" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="E38" s="64" t="s">
+      <c r="E38" s="47" t="s">
         <v>121</v>
       </c>
       <c r="I38" s="13"/>
@@ -3412,7 +3419,7 @@
       <c r="AH38" s="1"/>
     </row>
     <row r="39" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="66">
+      <c r="A39" s="49">
         <v>45664</v>
       </c>
       <c r="B39" s="7" t="s">
@@ -3424,7 +3431,7 @@
       <c r="D39" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="E39" s="64" t="s">
+      <c r="E39" s="47" t="s">
         <v>125</v>
       </c>
       <c r="I39" s="13"/>
@@ -3455,7 +3462,7 @@
       <c r="AH39" s="1"/>
     </row>
     <row r="40" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="66">
+      <c r="A40" s="49">
         <v>45695</v>
       </c>
       <c r="B40" s="7" t="s">
@@ -3467,7 +3474,7 @@
       <c r="D40" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="E40" s="64" t="s">
+      <c r="E40" s="47" t="s">
         <v>129</v>
       </c>
       <c r="I40" s="13"/>
@@ -3498,7 +3505,7 @@
       <c r="AH40" s="1"/>
     </row>
     <row r="41" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="66">
+      <c r="A41" s="49">
         <v>45723</v>
       </c>
       <c r="B41" s="7" t="s">
@@ -3510,7 +3517,7 @@
       <c r="D41" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="E41" s="64" t="s">
+      <c r="E41" s="47" t="s">
         <v>133</v>
       </c>
       <c r="F41" s="14"/>
@@ -3544,7 +3551,7 @@
       <c r="AH41" s="1"/>
     </row>
     <row r="42" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="63">
+      <c r="A42" s="46">
         <v>8</v>
       </c>
       <c r="B42" s="7" t="s">
@@ -3556,7 +3563,7 @@
       <c r="D42" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="E42" s="64" t="s">
+      <c r="E42" s="47" t="s">
         <v>137</v>
       </c>
       <c r="F42" s="14"/>
@@ -3571,26 +3578,26 @@
       <c r="O42" s="13"/>
       <c r="P42" s="13"/>
       <c r="Q42" s="2"/>
-      <c r="R42" s="37"/>
-      <c r="S42" s="38"/>
-      <c r="T42" s="38"/>
-      <c r="U42" s="38"/>
-      <c r="V42" s="38"/>
-      <c r="W42" s="38"/>
-      <c r="X42" s="38"/>
-      <c r="Y42" s="38"/>
-      <c r="Z42" s="38"/>
-      <c r="AA42" s="38"/>
-      <c r="AB42" s="38"/>
-      <c r="AC42" s="38"/>
-      <c r="AD42" s="38"/>
-      <c r="AE42" s="38"/>
-      <c r="AF42" s="38"/>
-      <c r="AG42" s="38"/>
-      <c r="AH42" s="39"/>
+      <c r="R42" s="56"/>
+      <c r="S42" s="57"/>
+      <c r="T42" s="57"/>
+      <c r="U42" s="57"/>
+      <c r="V42" s="57"/>
+      <c r="W42" s="57"/>
+      <c r="X42" s="57"/>
+      <c r="Y42" s="57"/>
+      <c r="Z42" s="57"/>
+      <c r="AA42" s="57"/>
+      <c r="AB42" s="57"/>
+      <c r="AC42" s="57"/>
+      <c r="AD42" s="57"/>
+      <c r="AE42" s="57"/>
+      <c r="AF42" s="57"/>
+      <c r="AG42" s="57"/>
+      <c r="AH42" s="58"/>
     </row>
     <row r="43" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="59"/>
+      <c r="A43" s="42"/>
       <c r="B43" s="8" t="s">
         <v>138</v>
       </c>
@@ -3598,7 +3605,7 @@
         <v>139</v>
       </c>
       <c r="D43" s="16"/>
-      <c r="E43" s="67"/>
+      <c r="E43" s="50"/>
       <c r="F43" s="13"/>
       <c r="G43" s="13"/>
       <c r="H43" s="13"/>
@@ -3611,26 +3618,26 @@
       <c r="O43" s="13"/>
       <c r="P43" s="13"/>
       <c r="Q43" s="2"/>
-      <c r="R43" s="37"/>
-      <c r="S43" s="38"/>
-      <c r="T43" s="38"/>
-      <c r="U43" s="38"/>
-      <c r="V43" s="38"/>
-      <c r="W43" s="38"/>
-      <c r="X43" s="38"/>
-      <c r="Y43" s="38"/>
-      <c r="Z43" s="38"/>
-      <c r="AA43" s="38"/>
-      <c r="AB43" s="38"/>
-      <c r="AC43" s="38"/>
-      <c r="AD43" s="38"/>
-      <c r="AE43" s="38"/>
-      <c r="AF43" s="38"/>
-      <c r="AG43" s="38"/>
-      <c r="AH43" s="39"/>
+      <c r="R43" s="56"/>
+      <c r="S43" s="57"/>
+      <c r="T43" s="57"/>
+      <c r="U43" s="57"/>
+      <c r="V43" s="57"/>
+      <c r="W43" s="57"/>
+      <c r="X43" s="57"/>
+      <c r="Y43" s="57"/>
+      <c r="Z43" s="57"/>
+      <c r="AA43" s="57"/>
+      <c r="AB43" s="57"/>
+      <c r="AC43" s="57"/>
+      <c r="AD43" s="57"/>
+      <c r="AE43" s="57"/>
+      <c r="AF43" s="57"/>
+      <c r="AG43" s="57"/>
+      <c r="AH43" s="58"/>
     </row>
     <row r="44" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="59"/>
+      <c r="A44" s="42"/>
       <c r="B44" s="7" t="s">
         <v>140</v>
       </c>
@@ -3638,7 +3645,7 @@
         <v>141</v>
       </c>
       <c r="D44" s="16"/>
-      <c r="E44" s="67"/>
+      <c r="E44" s="50"/>
       <c r="F44" s="14"/>
       <c r="G44" s="14"/>
       <c r="H44" s="14"/>
@@ -3651,26 +3658,26 @@
       <c r="O44" s="14"/>
       <c r="P44" s="14"/>
       <c r="Q44" s="2"/>
-      <c r="R44" s="37"/>
-      <c r="S44" s="38"/>
-      <c r="T44" s="38"/>
-      <c r="U44" s="38"/>
-      <c r="V44" s="38"/>
-      <c r="W44" s="38"/>
-      <c r="X44" s="38"/>
-      <c r="Y44" s="38"/>
-      <c r="Z44" s="38"/>
-      <c r="AA44" s="38"/>
-      <c r="AB44" s="38"/>
-      <c r="AC44" s="38"/>
-      <c r="AD44" s="38"/>
-      <c r="AE44" s="38"/>
-      <c r="AF44" s="38"/>
-      <c r="AG44" s="38"/>
-      <c r="AH44" s="39"/>
+      <c r="R44" s="56"/>
+      <c r="S44" s="57"/>
+      <c r="T44" s="57"/>
+      <c r="U44" s="57"/>
+      <c r="V44" s="57"/>
+      <c r="W44" s="57"/>
+      <c r="X44" s="57"/>
+      <c r="Y44" s="57"/>
+      <c r="Z44" s="57"/>
+      <c r="AA44" s="57"/>
+      <c r="AB44" s="57"/>
+      <c r="AC44" s="57"/>
+      <c r="AD44" s="57"/>
+      <c r="AE44" s="57"/>
+      <c r="AF44" s="57"/>
+      <c r="AG44" s="57"/>
+      <c r="AH44" s="58"/>
     </row>
     <row r="45" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="59"/>
+      <c r="A45" s="42"/>
       <c r="B45" s="8" t="s">
         <v>142</v>
       </c>
@@ -3678,7 +3685,7 @@
         <v>143</v>
       </c>
       <c r="D45" s="16"/>
-      <c r="E45" s="67"/>
+      <c r="E45" s="50"/>
       <c r="F45" s="14"/>
       <c r="G45" s="14"/>
       <c r="H45" s="14"/>
@@ -3710,7 +3717,7 @@
       <c r="AH45" s="1"/>
     </row>
     <row r="46" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="59"/>
+      <c r="A46" s="42"/>
       <c r="B46" s="27" t="s">
         <v>144</v>
       </c>
@@ -3718,7 +3725,7 @@
         <v>145</v>
       </c>
       <c r="D46" s="16"/>
-      <c r="E46" s="67"/>
+      <c r="E46" s="50"/>
       <c r="F46" s="14"/>
       <c r="G46" s="14"/>
       <c r="H46" s="14"/>
@@ -3750,13 +3757,13 @@
       <c r="AH46" s="1"/>
     </row>
     <row r="47" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="59"/>
+      <c r="A47" s="42"/>
       <c r="B47" s="30" t="s">
         <v>146</v>
       </c>
       <c r="C47" s="31"/>
       <c r="D47" s="25"/>
-      <c r="E47" s="68"/>
+      <c r="E47" s="51"/>
       <c r="I47" s="14"/>
       <c r="J47" s="14"/>
       <c r="K47" s="14"/>
@@ -3785,13 +3792,13 @@
       <c r="AH47" s="1"/>
     </row>
     <row r="48" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="59"/>
+      <c r="A48" s="42"/>
       <c r="B48" s="28" t="s">
         <v>147</v>
       </c>
       <c r="C48" s="19"/>
       <c r="D48" s="19"/>
-      <c r="E48" s="60"/>
+      <c r="E48" s="43"/>
       <c r="I48" s="14"/>
       <c r="J48" s="14"/>
       <c r="K48" s="14"/>
@@ -3820,7 +3827,7 @@
       <c r="AH48" s="1"/>
     </row>
     <row r="49" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="59"/>
+      <c r="A49" s="42"/>
       <c r="B49" s="32" t="s">
         <v>148</v>
       </c>
@@ -3828,7 +3835,7 @@
         <v>149</v>
       </c>
       <c r="D49" s="34"/>
-      <c r="E49" s="69"/>
+      <c r="E49" s="52"/>
       <c r="I49" s="14"/>
       <c r="J49" s="14"/>
       <c r="K49" s="14"/>
@@ -3857,7 +3864,7 @@
       <c r="AH49" s="1"/>
     </row>
     <row r="50" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="70"/>
+      <c r="A50" s="53"/>
       <c r="B50" s="11" t="s">
         <v>150</v>
       </c>
@@ -3865,7 +3872,7 @@
         <v>151</v>
       </c>
       <c r="D50" s="16"/>
-      <c r="E50" s="67"/>
+      <c r="E50" s="50"/>
       <c r="I50" s="14"/>
       <c r="J50" s="14"/>
       <c r="K50" s="14"/>
@@ -3894,7 +3901,7 @@
       <c r="AH50" s="1"/>
     </row>
     <row r="51" spans="1:34" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="70"/>
+      <c r="A51" s="53"/>
       <c r="B51" s="11" t="s">
         <v>152</v>
       </c>
@@ -3902,7 +3909,7 @@
         <v>153</v>
       </c>
       <c r="D51" s="16"/>
-      <c r="E51" s="67"/>
+      <c r="E51" s="50"/>
       <c r="I51" s="14"/>
       <c r="J51" s="14"/>
       <c r="K51" s="14"/>
@@ -3931,7 +3938,7 @@
       <c r="AH51" s="1"/>
     </row>
     <row r="52" spans="1:34" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="71"/>
+      <c r="A52" s="54"/>
       <c r="B52" s="29" t="s">
         <v>154</v>
       </c>
@@ -3939,7 +3946,7 @@
         <v>155</v>
       </c>
       <c r="D52" s="25"/>
-      <c r="E52" s="68"/>
+      <c r="E52" s="51"/>
       <c r="I52" s="14"/>
       <c r="J52" s="14"/>
       <c r="K52" s="14"/>
@@ -3968,13 +3975,13 @@
       <c r="AH52" s="1"/>
     </row>
     <row r="53" spans="1:34" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="72" t="s">
+      <c r="A53" s="76" t="s">
         <v>156</v>
       </c>
-      <c r="B53" s="44"/>
-      <c r="C53" s="44"/>
-      <c r="D53" s="44"/>
-      <c r="E53" s="73"/>
+      <c r="B53" s="77"/>
+      <c r="C53" s="77"/>
+      <c r="D53" s="77"/>
+      <c r="E53" s="78"/>
       <c r="F53" s="13"/>
       <c r="G53" s="13"/>
       <c r="H53" s="13"/>
@@ -4006,15 +4013,15 @@
       <c r="AH53" s="1"/>
     </row>
     <row r="54" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="74"/>
-      <c r="B54" s="45"/>
-      <c r="C54" s="45"/>
-      <c r="D54" s="45"/>
-      <c r="E54" s="75"/>
+      <c r="A54" s="79"/>
+      <c r="B54" s="80"/>
+      <c r="C54" s="80"/>
+      <c r="D54" s="80"/>
+      <c r="E54" s="81"/>
       <c r="F54" s="14"/>
       <c r="G54" s="14"/>
       <c r="H54" s="14"/>
-      <c r="I54" s="14"/>
+      <c r="I54" s="88"/>
       <c r="J54" s="14"/>
       <c r="K54" s="14"/>
       <c r="L54" s="14"/>
@@ -4042,11 +4049,11 @@
       <c r="AH54" s="1"/>
     </row>
     <row r="55" spans="1:34" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="76"/>
-      <c r="B55" s="46"/>
-      <c r="C55" s="46"/>
-      <c r="D55" s="46"/>
-      <c r="E55" s="77"/>
+      <c r="A55" s="82"/>
+      <c r="B55" s="83"/>
+      <c r="C55" s="83"/>
+      <c r="D55" s="83"/>
+      <c r="E55" s="84"/>
       <c r="F55" s="13"/>
       <c r="G55" s="13"/>
       <c r="H55" s="13"/>
@@ -4078,13 +4085,13 @@
       <c r="AH55" s="1"/>
     </row>
     <row r="56" spans="1:34" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="78" t="s">
+      <c r="A56" s="85" t="s">
         <v>157</v>
       </c>
-      <c r="B56" s="47"/>
-      <c r="C56" s="47"/>
-      <c r="D56" s="47"/>
-      <c r="E56" s="79"/>
+      <c r="B56" s="86"/>
+      <c r="C56" s="86"/>
+      <c r="D56" s="86"/>
+      <c r="E56" s="87"/>
       <c r="F56" s="13"/>
       <c r="G56" s="13"/>
       <c r="H56" s="13"/>
@@ -4116,13 +4123,13 @@
       <c r="AH56" s="1"/>
     </row>
     <row r="57" spans="1:34" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="80" t="s">
+      <c r="A57" s="67" t="s">
         <v>158</v>
       </c>
-      <c r="B57" s="42"/>
-      <c r="C57" s="42"/>
-      <c r="D57" s="42"/>
-      <c r="E57" s="81"/>
+      <c r="B57" s="68"/>
+      <c r="C57" s="68"/>
+      <c r="D57" s="68"/>
+      <c r="E57" s="69"/>
       <c r="F57" s="13"/>
       <c r="G57" s="13"/>
       <c r="H57" s="13"/>
@@ -4154,11 +4161,11 @@
       <c r="AH57" s="1"/>
     </row>
     <row r="58" spans="1:34" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="82"/>
-      <c r="B58" s="43"/>
-      <c r="C58" s="43"/>
-      <c r="D58" s="43"/>
-      <c r="E58" s="83"/>
+      <c r="A58" s="70"/>
+      <c r="B58" s="71"/>
+      <c r="C58" s="71"/>
+      <c r="D58" s="71"/>
+      <c r="E58" s="72"/>
       <c r="F58" s="14"/>
       <c r="G58" s="14"/>
       <c r="H58" s="14"/>
@@ -4190,11 +4197,11 @@
       <c r="AH58" s="1"/>
     </row>
     <row r="59" spans="1:34" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="82"/>
-      <c r="B59" s="43"/>
-      <c r="C59" s="43"/>
-      <c r="D59" s="43"/>
-      <c r="E59" s="83"/>
+      <c r="A59" s="70"/>
+      <c r="B59" s="71"/>
+      <c r="C59" s="71"/>
+      <c r="D59" s="71"/>
+      <c r="E59" s="72"/>
       <c r="F59" s="14"/>
       <c r="G59" s="14"/>
       <c r="H59" s="14"/>
@@ -4225,12 +4232,12 @@
       <c r="AG59" s="1"/>
       <c r="AH59" s="1"/>
     </row>
-    <row r="60" spans="1:34" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="84"/>
-      <c r="B60" s="85"/>
-      <c r="C60" s="85"/>
-      <c r="D60" s="85"/>
-      <c r="E60" s="86"/>
+    <row r="60" spans="1:34" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="73"/>
+      <c r="B60" s="74"/>
+      <c r="C60" s="74"/>
+      <c r="D60" s="74"/>
+      <c r="E60" s="75"/>
       <c r="F60" s="13"/>
       <c r="G60" s="13"/>
       <c r="H60" s="13"/>
@@ -4334,11 +4341,11 @@
       <c r="AH62" s="1"/>
     </row>
     <row r="63" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="88"/>
-      <c r="B63" s="89"/>
-      <c r="C63" s="87"/>
-      <c r="D63" s="89"/>
-      <c r="E63" s="89"/>
+      <c r="A63" s="55"/>
+      <c r="B63" s="34"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="34"/>
+      <c r="E63" s="34"/>
       <c r="F63" s="13"/>
       <c r="G63" s="13"/>
       <c r="H63" s="13"/>
@@ -4370,13 +4377,13 @@
       <c r="AH63" s="1"/>
     </row>
     <row r="64" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="40" t="s">
+      <c r="A64" s="65" t="s">
         <v>159</v>
       </c>
-      <c r="B64" s="41"/>
-      <c r="C64" s="41"/>
-      <c r="D64" s="41"/>
-      <c r="E64" s="41"/>
+      <c r="B64" s="66"/>
+      <c r="C64" s="66"/>
+      <c r="D64" s="66"/>
+      <c r="E64" s="66"/>
       <c r="F64" s="5"/>
       <c r="G64" s="5"/>
       <c r="H64" s="5"/>
@@ -38177,6 +38184,20 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="R42:AH42"/>
+    <mergeCell ref="A64:E64"/>
+    <mergeCell ref="A57:E60"/>
+    <mergeCell ref="A53:E55"/>
+    <mergeCell ref="A56:E56"/>
+    <mergeCell ref="R43:AH43"/>
+    <mergeCell ref="R44:AH44"/>
+    <mergeCell ref="R24:AH24"/>
+    <mergeCell ref="R25:AH25"/>
+    <mergeCell ref="R26:AH26"/>
+    <mergeCell ref="R23:AH23"/>
+    <mergeCell ref="R17:AH17"/>
+    <mergeCell ref="R18:AH18"/>
+    <mergeCell ref="R19:AH19"/>
     <mergeCell ref="R15:AH15"/>
     <mergeCell ref="R16:AH16"/>
     <mergeCell ref="G7:I7"/>
@@ -38190,20 +38211,6 @@
     <mergeCell ref="R13:AH13"/>
     <mergeCell ref="R11:AH11"/>
     <mergeCell ref="R12:AH12"/>
-    <mergeCell ref="R24:AH24"/>
-    <mergeCell ref="R25:AH25"/>
-    <mergeCell ref="R26:AH26"/>
-    <mergeCell ref="R23:AH23"/>
-    <mergeCell ref="R17:AH17"/>
-    <mergeCell ref="R18:AH18"/>
-    <mergeCell ref="R19:AH19"/>
-    <mergeCell ref="R42:AH42"/>
-    <mergeCell ref="A64:E64"/>
-    <mergeCell ref="A57:E60"/>
-    <mergeCell ref="A53:E55"/>
-    <mergeCell ref="A56:E56"/>
-    <mergeCell ref="R43:AH43"/>
-    <mergeCell ref="R44:AH44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>